<commit_message>
Why does Line 80 not show all of the data in class_list?
</commit_message>
<xml_diff>
--- a/List of Classes.xlsx
+++ b/List of Classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihaowang/PycharmProjects/Class-Recommendations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AA0B7C-F078-5B4A-9E1D-A342143BD6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A57A574-38B2-F646-AA0E-20C20D554070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{CA0135AE-1A56-214D-AEB7-D881AE2C68B6}"/>
+    <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{CA0135AE-1A56-214D-AEB7-D881AE2C68B6}"/>
   </bookViews>
   <sheets>
     <sheet name="HASS Classes" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D2" sqref="D2:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
<a> </a> on line 17
</commit_message>
<xml_diff>
--- a/List of Classes.xlsx
+++ b/List of Classes.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihaowang/PycharmProjects/Class-Recommendations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A57A574-38B2-F646-AA0E-20C20D554070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB63885-C796-E84A-B75C-8E00349E457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{CA0135AE-1A56-214D-AEB7-D881AE2C68B6}"/>
+    <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17420" xr2:uid="{CA0135AE-1A56-214D-AEB7-D881AE2C68B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="HASS Classes" sheetId="1" r:id="rId1"/>
-    <sheet name="Course 6 Classes" sheetId="2" r:id="rId2"/>
+    <sheet name="Course 6 Classes" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Course Number</t>
   </si>
@@ -459,50 +458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76CBFFA-1226-8145-A297-D8504910409C}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963A7216-AD8D-E14A-935E-E2E2FCB21451}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +647,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A5:A6" numberStoredAsText="1"/>
+    <ignoredError sqref="A5:A7 A8:A15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>